<commit_message>
Aktualizacja dokumentacji podłączenia kanałów analogowych i cyfrowych w dokumentacji
</commit_message>
<xml_diff>
--- a/Dokumentacja/opis we_wy karty 6210.xlsx
+++ b/Dokumentacja/opis we_wy karty 6210.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Cyfrowe</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>Chan 8 IN</t>
-  </si>
-  <si>
-    <t>Ohm IN (0V - 3,5V L - h)</t>
   </si>
   <si>
     <t>Digital 1 IN (/16)</t>
@@ -214,10 +211,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,7 +520,7 @@
   <dimension ref="B4:AH7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL7" sqref="AL7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,42 +530,42 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="S4" s="1" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="S4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
     </row>
     <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -668,167 +665,164 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:34" s="2" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="2:34" s="1" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="S6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="U6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="V6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="W6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="X6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Y6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="Z6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AA6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AB6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AC6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AD6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE6" s="2" t="s">
+      <c r="AE6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AF6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG6" s="2" t="s">
+      <c r="AG6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH6" s="2" t="s">
+      <c r="AH6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:34" s="2" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="2:34" s="1" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="S7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="T7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T7" s="2" t="s">
+      <c r="AF7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="U7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V7" s="2" t="s">
+      <c r="AG7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH7" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG7" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>